<commit_message>
HAHAHA Viktor får mergefejl
</commit_message>
<xml_diff>
--- a/Lab-Scale-Group65/Rå-Målinger.kinda-trash.xlsx
+++ b/Lab-Scale-Group65/Rå-Målinger.kinda-trash.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktor\Documents\GitHub\GFV\Lab-Scale-Group65\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anton\OneDrive - Aarhus universitet\3. semester\GFV\GFV - LAB\Lab-Scale-Group65\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87788AD-70F3-45D3-97B1-E4073B4DED53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="6_{C28A6CEC-0FD4-4BD9-AC2A-9608EF0B0942}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{A8F3F9C1-B63D-42DE-B474-39E1C2E8C240}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4581D2D8-8E95-4720-8671-B7B6BA209B26}"/>
+    <workbookView xWindow="30" yWindow="600" windowWidth="28770" windowHeight="15600" xr2:uid="{4581D2D8-8E95-4720-8671-B7B6BA209B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Indledende" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
-    <t>vægt</t>
-  </si>
-  <si>
     <t>hex</t>
-  </si>
-  <si>
-    <t>dec</t>
   </si>
   <si>
     <t>7cc</t>
@@ -230,6 +224,12 @@
   <si>
     <t>ZD i proc</t>
   </si>
+  <si>
+    <t>Belastning på vægten [g]</t>
+  </si>
+  <si>
+    <t>Analog måling</t>
+  </si>
 </sst>
 </file>
 
@@ -290,7 +290,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -322,7 +322,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="da-DK"/>
-              <a:t>titulær diagrammius</a:t>
+              <a:t>Graf over belastningen på vægten sammenlignet med målt analoge data fra strain gaugen</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -352,7 +352,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -405,8 +405,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.47487518054680239"/>
-                  <c:y val="-0.12325419928360554"/>
+                  <c:x val="0.29037021177911282"/>
+                  <c:y val="-9.0767813315370982E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -434,57 +434,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="LID4096"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:prstDash val="dash"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.48795547452236326"/>
-                  <c:y val="3.2139164247224107E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="LID4096"/>
+                  <a:endParaRPr lang="da-DK"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -749,6 +699,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Belastning på vægten [g]</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="da-DK" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -783,7 +795,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="592311200"/>
@@ -812,6 +824,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Analog måling</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -840,7 +907,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="592315136"/>
@@ -882,7 +949,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -919,13 +986,13 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0" l="0" r="0" t="0" header="0" footer="0"/>
+    <c:pageSetup paperSize="9" orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -933,7 +1000,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -995,7 +1062,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1611,7 +1678,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783260272"/>
@@ -1674,7 +1741,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783261584"/>
@@ -1716,7 +1783,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1753,7 +1820,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1767,7 +1834,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1829,7 +1896,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2061,7 +2128,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="da-DK"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2099,7 +2166,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783285208"/>
@@ -2186,7 +2253,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="da-DK"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2218,7 +2285,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="684562768"/>
@@ -2288,7 +2355,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="LID4096"/>
+              <a:endParaRPr lang="da-DK"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2320,7 +2387,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="680668720"/>
@@ -2338,6 +2405,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="680669704"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2378,7 +2446,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2415,7 +2483,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2429,7 +2497,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2466,7 +2534,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2627,7 +2695,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783258304"/>
@@ -2686,7 +2754,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783258632"/>
@@ -2734,7 +2802,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2748,7 +2816,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2785,7 +2853,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2946,7 +3014,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783258304"/>
@@ -3005,7 +3073,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="LID4096"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="783258632"/>
@@ -3053,7 +3121,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="LID4096"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5809,16 +5877,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>276224</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6008,7 +6076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -6304,26 +6372,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420FC2B5-1126-42BE-85AE-0DF4ACA84898}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="D1" t="str">
+        <f>CONCATENATE(A1," &amp; ",B1, " \\ \hline")</f>
+        <v>Belastning på vægten [g] &amp; Analog måling \\ \hline</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -6334,8 +6404,12 @@
       <c r="C2" s="1">
         <v>443</v>
       </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D37" si="1">CONCATENATE(A2," &amp; ",B2, " \\ \hline")</f>
+        <v>0 &amp; 1091 \\ \hline</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>151</v>
       </c>
@@ -6344,10 +6418,14 @@
         <v>1119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>151 &amp; 1119 \\ \hline</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>302</v>
       </c>
@@ -6358,8 +6436,12 @@
       <c r="C4" s="1">
         <v>483</v>
       </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>302 &amp; 1155 \\ \hline</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>453</v>
       </c>
@@ -6368,10 +6450,14 @@
         <v>1189</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>453 &amp; 1189 \\ \hline</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>604</v>
       </c>
@@ -6380,10 +6466,14 @@
         <v>1222</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>604 &amp; 1222 \\ \hline</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>755</v>
       </c>
@@ -6392,10 +6482,14 @@
         <v>1252</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>755 &amp; 1252 \\ \hline</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -6404,10 +6498,14 @@
         <v>1297</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>1000 &amp; 1297 \\ \hline</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1151</v>
       </c>
@@ -6416,10 +6514,14 @@
         <v>1325</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>1151 &amp; 1325 \\ \hline</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1302</v>
       </c>
@@ -6428,10 +6530,14 @@
         <v>1356</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>1302 &amp; 1356 \\ \hline</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1453</v>
       </c>
@@ -6440,10 +6546,14 @@
         <v>1383</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>1453 &amp; 1383 \\ \hline</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1604</v>
       </c>
@@ -6452,10 +6562,14 @@
         <v>1408</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>1604 &amp; 1408 \\ \hline</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1755</v>
       </c>
@@ -6464,10 +6578,14 @@
         <v>1469</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>1755 &amp; 1469 \\ \hline</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2000</v>
       </c>
@@ -6476,10 +6594,14 @@
         <v>1510</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>2000 &amp; 1510 \\ \hline</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2151</v>
       </c>
@@ -6488,10 +6610,14 @@
         <v>1539</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>2151 &amp; 1539 \\ \hline</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2302</v>
       </c>
@@ -6500,10 +6626,14 @@
         <v>1571</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>2302 &amp; 1571 \\ \hline</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2453</v>
       </c>
@@ -6512,10 +6642,14 @@
         <v>1594</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>2453 &amp; 1594 \\ \hline</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2604</v>
       </c>
@@ -6524,10 +6658,14 @@
         <v>1630</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>2604 &amp; 1630 \\ \hline</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2755</v>
       </c>
@@ -6536,10 +6674,14 @@
         <v>1657</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>2755 &amp; 1657 \\ \hline</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3000</v>
       </c>
@@ -6548,10 +6690,14 @@
         <v>1718</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>3000 &amp; 1718 \\ \hline</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3151</v>
       </c>
@@ -6560,10 +6706,14 @@
         <v>1753</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>3151 &amp; 1753 \\ \hline</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3302</v>
       </c>
@@ -6572,10 +6722,14 @@
         <v>1777</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>3302 &amp; 1777 \\ \hline</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3453</v>
       </c>
@@ -6584,10 +6738,14 @@
         <v>1811</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>3453 &amp; 1811 \\ \hline</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3604</v>
       </c>
@@ -6596,10 +6754,14 @@
         <v>1842</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>3604 &amp; 1842 \\ \hline</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3755</v>
       </c>
@@ -6608,10 +6770,14 @@
         <v>1873</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>3755 &amp; 1873 \\ \hline</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4000</v>
       </c>
@@ -6620,10 +6786,14 @@
         <v>1929</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>4000 &amp; 1929 \\ \hline</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4151</v>
       </c>
@@ -6632,10 +6802,14 @@
         <v>1959</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>4151 &amp; 1959 \\ \hline</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4302</v>
       </c>
@@ -6644,10 +6818,14 @@
         <v>1996</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>4302 &amp; 1996 \\ \hline</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4453</v>
       </c>
@@ -6656,10 +6834,14 @@
         <v>2025</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>4453 &amp; 2025 \\ \hline</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4604</v>
       </c>
@@ -6668,10 +6850,14 @@
         <v>2057</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>4604 &amp; 2057 \\ \hline</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4755</v>
       </c>
@@ -6680,10 +6866,14 @@
         <v>2094</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>4755 &amp; 2094 \\ \hline</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>5000</v>
       </c>
@@ -6692,10 +6882,14 @@
         <v>2141</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>5000 &amp; 2141 \\ \hline</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5151</v>
       </c>
@@ -6704,10 +6898,14 @@
         <v>2156</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>5151 &amp; 2156 \\ \hline</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5302</v>
       </c>
@@ -6716,10 +6914,14 @@
         <v>2167</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>5302 &amp; 2167 \\ \hline</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5453</v>
       </c>
@@ -6728,10 +6930,14 @@
         <v>2177</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>5453 &amp; 2177 \\ \hline</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5604</v>
       </c>
@@ -6740,10 +6946,14 @@
         <v>2184</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>5604 &amp; 2184 \\ \hline</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>5755</v>
       </c>
@@ -6752,12 +6962,17 @@
         <v>2188</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>5755 &amp; 2188 \\ \hline</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="150" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6773,19 +6988,19 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -7029,58 +7244,58 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
-      </c>
-      <c r="S1" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -7422,37 +7637,37 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
         <v>62</v>
-      </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -7577,7 +7792,7 @@
         <v>44.380000000000109</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M3:M7" si="3">L4/J4*100</f>
+        <f t="shared" ref="M4:M7" si="3">L4/J4*100</f>
         <v>2.2348788139732858</v>
       </c>
     </row>

</xml_diff>